<commit_message>
Update Sprint 1 Backlog v2.0.xlsx
</commit_message>
<xml_diff>
--- a/Sprint 1 Backlog v2.0.xlsx
+++ b/Sprint 1 Backlog v2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florinbordei/Documents/GitHub/SEP2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ledao\Project\SEP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F0169A8-3A9F-7842-8163-3E61A0172052}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8C265C-7B8A-4346-9683-E73FDB013939}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{4827F640-2CAA-B341-9D86-7CBD5337AD55}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4827F640-2CAA-B341-9D86-7CBD5337AD55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="153">
   <si>
     <t>Warehouse wants to provide inventory stock to HQ</t>
   </si>
@@ -484,6 +484,9 @@
   </si>
   <si>
     <t>Add Stock Item to Shop Inventory</t>
+  </si>
+  <si>
+    <t>Sprint 5 NEW - As a manager at the Shop I would like to delete stock item</t>
   </si>
 </sst>
 </file>
@@ -730,7 +733,43 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -742,55 +781,25 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -799,31 +808,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,10 +820,28 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1160,48 +1163,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CC97EA-6960-974F-BAE0-14E63826BEA4}">
   <dimension ref="A2:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60:E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="5" max="5" width="91.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" customWidth="1"/>
+    <col min="5" max="5" width="91.125" customWidth="1"/>
+    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1218,18 +1221,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="3">
         <v>16</v>
       </c>
@@ -1246,18 +1249,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="3">
         <v>10</v>
       </c>
@@ -1274,18 +1277,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="3">
         <v>8</v>
       </c>
@@ -1302,18 +1305,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="3">
         <v>6</v>
       </c>
@@ -1330,18 +1333,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="3">
         <v>8</v>
       </c>
@@ -1358,18 +1361,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="3">
         <v>8</v>
       </c>
@@ -1386,32 +1389,32 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+    <row r="12" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-    </row>
-    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1428,18 +1431,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="3">
         <v>16</v>
       </c>
@@ -1456,18 +1459,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="3">
         <v>10</v>
       </c>
@@ -1484,18 +1487,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>3</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="3">
         <v>8</v>
       </c>
@@ -1512,18 +1515,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="3">
         <v>6</v>
       </c>
@@ -1540,18 +1543,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>5</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="3">
         <v>8</v>
       </c>
@@ -1568,18 +1571,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="3">
         <v>8</v>
       </c>
@@ -1596,37 +1599,37 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-    </row>
-    <row r="23" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
       <c r="F23" s="2" t="s">
         <v>8</v>
       </c>
@@ -1643,18 +1646,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>1</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="3">
         <v>16</v>
       </c>
@@ -1669,18 +1672,18 @@
       </c>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
       <c r="F25" s="3">
         <v>10</v>
       </c>
@@ -1695,18 +1698,18 @@
       </c>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>3</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="3">
         <v>8</v>
       </c>
@@ -1721,18 +1724,18 @@
       </c>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>4</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
       <c r="F27" s="3">
         <v>6</v>
       </c>
@@ -1747,18 +1750,18 @@
       </c>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>5</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="3">
         <v>8</v>
       </c>
@@ -1773,18 +1776,18 @@
       </c>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>6</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="3">
         <v>8</v>
       </c>
@@ -1799,18 +1802,18 @@
       </c>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>7</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3" t="s">
@@ -1821,18 +1824,18 @@
       </c>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>8</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
@@ -1843,18 +1846,18 @@
       </c>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>9</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
@@ -1865,18 +1868,18 @@
       </c>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>10</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3" t="s">
@@ -1887,18 +1890,18 @@
       </c>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>11</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3" t="s">
@@ -1909,32 +1912,32 @@
       </c>
       <c r="J34" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A37" s="24" t="s">
+    <row r="37" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A37" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-    </row>
-    <row r="38" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+    </row>
+    <row r="38" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
       <c r="F38" s="2" t="s">
         <v>8</v>
       </c>
@@ -1951,16 +1954,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>1</v>
       </c>
       <c r="B39" s="3"/>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="28"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="23"/>
       <c r="F39" s="3"/>
       <c r="G39" s="14" t="s">
         <v>100</v>
@@ -1971,182 +1974,182 @@
       <c r="I39" s="4"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>2</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="28"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="23"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="4"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>3</v>
       </c>
       <c r="B41" s="3"/>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="28"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="4"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>4</v>
       </c>
       <c r="B42" s="3"/>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="28"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="23"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="4"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>5</v>
       </c>
       <c r="B43" s="3"/>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="D43" s="32"/>
-      <c r="E43" s="33"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="26"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="5"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>6</v>
       </c>
       <c r="B44" s="3"/>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="4"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>7</v>
       </c>
       <c r="B45" s="11"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="23"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="4"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>8</v>
       </c>
       <c r="B46" s="11"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="4"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>9</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="4"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>10</v>
       </c>
       <c r="B48" s="11"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="5"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>11</v>
       </c>
       <c r="B49" s="11"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="5"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="52" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A52" s="24" t="s">
+    <row r="52" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A52" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-    </row>
-    <row r="53" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="27"/>
+    </row>
+    <row r="53" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="25" t="s">
+      <c r="C53" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
       <c r="F53" s="2" t="s">
         <v>8</v>
       </c>
@@ -2163,16 +2166,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>1</v>
       </c>
       <c r="B54" s="3"/>
-      <c r="C54" s="26" t="s">
+      <c r="C54" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="27"/>
-      <c r="E54" s="28"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="23"/>
       <c r="F54" s="3"/>
       <c r="G54" s="14"/>
       <c r="H54" s="3" t="s">
@@ -2181,16 +2184,16 @@
       <c r="I54" s="4"/>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>2</v>
       </c>
       <c r="B55" s="3"/>
-      <c r="C55" s="26" t="s">
+      <c r="C55" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="27"/>
-      <c r="E55" s="28"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="23"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3" t="s">
@@ -2199,16 +2202,16 @@
       <c r="I55" s="4"/>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>3</v>
       </c>
       <c r="B56" s="3"/>
-      <c r="C56" s="26" t="s">
+      <c r="C56" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="D56" s="27"/>
-      <c r="E56" s="28"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="23"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3" t="s">
@@ -2217,16 +2220,16 @@
       <c r="I56" s="4"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>4</v>
       </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="D57" s="27"/>
-      <c r="E57" s="28"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="23"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3" t="s">
@@ -2235,16 +2238,16 @@
       <c r="I57" s="4"/>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>5</v>
       </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="31" t="s">
+      <c r="C58" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="D58" s="32"/>
-      <c r="E58" s="33"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="26"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3" t="s">
@@ -2253,99 +2256,142 @@
       <c r="I58" s="5"/>
       <c r="J58" s="3"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>6</v>
       </c>
       <c r="B59" s="3"/>
-      <c r="C59" s="26" t="s">
+      <c r="C59" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="D59" s="27"/>
-      <c r="E59" s="28"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="23"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="4"/>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>7</v>
       </c>
       <c r="B60" s="11"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
+      <c r="C60" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="4"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>8</v>
       </c>
       <c r="B61" s="11"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="29"/>
+      <c r="C61" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="4"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>9</v>
       </c>
       <c r="B62" s="11"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="4"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>10</v>
       </c>
       <c r="B63" s="11"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="5"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>11</v>
       </c>
       <c r="B64" s="11"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="5"/>
       <c r="J64" s="3"/>
     </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C46:E46"/>
     <mergeCell ref="C62:E62"/>
     <mergeCell ref="C63:E63"/>
     <mergeCell ref="C64:E64"/>
@@ -2362,45 +2408,6 @@
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="A37:J37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="A22:J22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2414,82 +2421,82 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
       <c r="J4" t="s">
         <v>50</v>
       </c>
       <c r="K4" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="35" t="s">
+      <c r="N4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
       <c r="J5" s="6">
         <v>5</v>
       </c>
@@ -2499,31 +2506,31 @@
       <c r="M5">
         <v>1</v>
       </c>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
       <c r="J6" s="6">
         <v>5</v>
       </c>
@@ -2533,31 +2540,31 @@
       <c r="M6">
         <v>2</v>
       </c>
-      <c r="N6" s="38" t="s">
+      <c r="N6" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
       <c r="J7" s="6">
         <v>4</v>
       </c>
@@ -2567,31 +2574,31 @@
       <c r="M7">
         <v>3</v>
       </c>
-      <c r="N7" s="38" t="s">
+      <c r="N7" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
       <c r="J8" s="6">
         <v>4</v>
       </c>
@@ -2601,31 +2608,31 @@
       <c r="M8">
         <v>4</v>
       </c>
-      <c r="N8" s="38" t="s">
+      <c r="N8" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
       <c r="J9" s="6">
         <v>4</v>
       </c>
@@ -2635,18 +2642,18 @@
       <c r="M9">
         <v>5</v>
       </c>
-      <c r="N9" s="38" t="s">
+      <c r="N9" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2680,7 +2687,7 @@
       <c r="T10" s="36"/>
       <c r="U10" s="36"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2711,7 +2718,7 @@
       <c r="T11" s="34"/>
       <c r="U11" s="34"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2742,7 +2749,7 @@
       <c r="T12" s="34"/>
       <c r="U12" s="34"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2773,7 +2780,7 @@
       <c r="T13" s="34"/>
       <c r="U13" s="34"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2804,7 +2811,7 @@
       <c r="T14" s="34"/>
       <c r="U14" s="34"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2835,7 +2842,7 @@
       <c r="T15" s="34"/>
       <c r="U15" s="34"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2866,7 +2873,7 @@
       <c r="T16" s="34"/>
       <c r="U16" s="34"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2897,7 +2904,7 @@
       <c r="T17" s="34"/>
       <c r="U17" s="34"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2928,7 +2935,7 @@
       <c r="T18" s="34"/>
       <c r="U18" s="34"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2962,7 +2969,7 @@
       <c r="T19" s="36"/>
       <c r="U19" s="36"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2985,18 +2992,18 @@
       <c r="M20">
         <v>17</v>
       </c>
-      <c r="N20" s="39" t="s">
+      <c r="N20" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="39"/>
-      <c r="U20" s="39"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="37"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -3016,18 +3023,18 @@
       <c r="M21">
         <v>18</v>
       </c>
-      <c r="N21" s="40" t="s">
+      <c r="N21" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="40"/>
-      <c r="S21" s="40"/>
-      <c r="T21" s="40"/>
-      <c r="U21" s="40"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -3050,49 +3057,49 @@
       <c r="M22">
         <v>19</v>
       </c>
-      <c r="N22" s="39" t="s">
+      <c r="N22" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="O22" s="39"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="39"/>
-      <c r="R22" s="39"/>
-      <c r="S22" s="39"/>
-      <c r="T22" s="39"/>
-      <c r="U22" s="39"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
       <c r="J23" s="6">
         <v>4</v>
       </c>
       <c r="M23">
         <v>20</v>
       </c>
-      <c r="N23" s="37" t="s">
+      <c r="N23" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="37"/>
-      <c r="T23" s="37"/>
-      <c r="U23" s="37"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -3123,7 +3130,7 @@
       <c r="T24" s="34"/>
       <c r="U24" s="34"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -3154,7 +3161,7 @@
       <c r="T25" s="34"/>
       <c r="U25" s="34"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -3185,7 +3192,7 @@
       <c r="T26" s="34"/>
       <c r="U26" s="34"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -3216,7 +3223,7 @@
       <c r="T27" s="34"/>
       <c r="U27" s="34"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -3247,7 +3254,7 @@
       <c r="T28" s="34"/>
       <c r="U28" s="34"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -3278,7 +3285,7 @@
       <c r="T29" s="34"/>
       <c r="U29" s="34"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -3309,7 +3316,7 @@
       <c r="T30" s="34"/>
       <c r="U30" s="34"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -3340,7 +3347,7 @@
       <c r="T31" s="34"/>
       <c r="U31" s="34"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
       <c r="D32" s="34"/>
@@ -3363,7 +3370,7 @@
       <c r="T32" s="34"/>
       <c r="U32" s="34"/>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" s="34"/>
       <c r="C33" s="34"/>
       <c r="D33" s="34"/>
@@ -3375,18 +3382,18 @@
       <c r="M33">
         <v>30</v>
       </c>
-      <c r="N33" s="41" t="s">
+      <c r="N33" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="O33" s="41"/>
-      <c r="P33" s="41"/>
-      <c r="Q33" s="41"/>
-      <c r="R33" s="41"/>
-      <c r="S33" s="41"/>
-      <c r="T33" s="41"/>
-      <c r="U33" s="41"/>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O33" s="35"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="35"/>
+      <c r="U33" s="35"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34" s="34"/>
       <c r="C34" s="34"/>
       <c r="D34" s="34"/>
@@ -3398,18 +3405,18 @@
       <c r="M34">
         <v>31</v>
       </c>
-      <c r="N34" s="41" t="s">
+      <c r="N34" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="O34" s="41"/>
-      <c r="P34" s="41"/>
-      <c r="Q34" s="41"/>
-      <c r="R34" s="41"/>
-      <c r="S34" s="41"/>
-      <c r="T34" s="41"/>
-      <c r="U34" s="41"/>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O34" s="35"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="34"/>
       <c r="C35" s="34"/>
       <c r="D35" s="34"/>
@@ -3421,168 +3428,168 @@
       <c r="M35">
         <v>32</v>
       </c>
-      <c r="N35" s="41" t="s">
+      <c r="N35" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="O35" s="41"/>
-      <c r="P35" s="41"/>
-      <c r="Q35" s="41"/>
-      <c r="R35" s="41"/>
-      <c r="S35" s="41"/>
-      <c r="T35" s="41"/>
-      <c r="U35" s="41"/>
-    </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O35" s="35"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
+      <c r="S35" s="35"/>
+      <c r="T35" s="35"/>
+      <c r="U35" s="35"/>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M36">
         <v>33</v>
       </c>
-      <c r="N36" s="41" t="s">
+      <c r="N36" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="41"/>
-      <c r="S36" s="41"/>
-      <c r="T36" s="41"/>
-      <c r="U36" s="41"/>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O36" s="35"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="35"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="35"/>
+      <c r="U36" s="35"/>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M37">
         <v>34</v>
       </c>
-      <c r="N37" s="41" t="s">
+      <c r="N37" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="O37" s="41"/>
-      <c r="P37" s="41"/>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="41"/>
-      <c r="S37" s="41"/>
-      <c r="T37" s="41"/>
-      <c r="U37" s="41"/>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
+      <c r="S37" s="35"/>
+      <c r="T37" s="35"/>
+      <c r="U37" s="35"/>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M38">
         <v>35</v>
       </c>
-      <c r="N38" s="41" t="s">
+      <c r="N38" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="41"/>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O38" s="35"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="35"/>
+      <c r="S38" s="35"/>
+      <c r="T38" s="35"/>
+      <c r="U38" s="35"/>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M39">
         <v>36</v>
       </c>
-      <c r="N39" s="41" t="s">
+      <c r="N39" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="O39" s="41"/>
-      <c r="P39" s="41"/>
-      <c r="Q39" s="41"/>
-      <c r="R39" s="41"/>
-      <c r="S39" s="41"/>
-      <c r="T39" s="41"/>
-      <c r="U39" s="41"/>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O39" s="35"/>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
+      <c r="R39" s="35"/>
+      <c r="S39" s="35"/>
+      <c r="T39" s="35"/>
+      <c r="U39" s="35"/>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M40">
         <v>37</v>
       </c>
-      <c r="N40" s="41" t="s">
+      <c r="N40" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="O40" s="41"/>
-      <c r="P40" s="41"/>
-      <c r="Q40" s="41"/>
-      <c r="R40" s="41"/>
-      <c r="S40" s="41"/>
-      <c r="T40" s="41"/>
-      <c r="U40" s="41"/>
-    </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="35"/>
+      <c r="U40" s="35"/>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M41">
         <v>38</v>
       </c>
-      <c r="N41" s="41" t="s">
+      <c r="N41" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="O41" s="41"/>
-      <c r="P41" s="41"/>
-      <c r="Q41" s="41"/>
-      <c r="R41" s="41"/>
-      <c r="S41" s="41"/>
-      <c r="T41" s="41"/>
-      <c r="U41" s="41"/>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
+      <c r="S41" s="35"/>
+      <c r="T41" s="35"/>
+      <c r="U41" s="35"/>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M42">
         <v>39</v>
       </c>
-      <c r="N42" s="41" t="s">
+      <c r="N42" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="O42" s="41"/>
-      <c r="P42" s="41"/>
-      <c r="Q42" s="41"/>
-      <c r="R42" s="41"/>
-      <c r="S42" s="41"/>
-      <c r="T42" s="41"/>
-      <c r="U42" s="41"/>
-    </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O42" s="35"/>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="35"/>
+      <c r="R42" s="35"/>
+      <c r="S42" s="35"/>
+      <c r="T42" s="35"/>
+      <c r="U42" s="35"/>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M43">
         <v>40</v>
       </c>
-      <c r="N43" s="41" t="s">
+      <c r="N43" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="O43" s="41"/>
-      <c r="P43" s="41"/>
-      <c r="Q43" s="41"/>
-      <c r="R43" s="41"/>
-      <c r="S43" s="41"/>
-      <c r="T43" s="41"/>
-      <c r="U43" s="41"/>
-    </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O43" s="35"/>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="35"/>
+      <c r="S43" s="35"/>
+      <c r="T43" s="35"/>
+      <c r="U43" s="35"/>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M44">
         <v>41</v>
       </c>
-      <c r="N44" s="41" t="s">
+      <c r="N44" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="O44" s="41"/>
-      <c r="P44" s="41"/>
-      <c r="Q44" s="41"/>
-      <c r="R44" s="41"/>
-      <c r="S44" s="41"/>
-      <c r="T44" s="41"/>
-      <c r="U44" s="41"/>
-    </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O44" s="35"/>
+      <c r="P44" s="35"/>
+      <c r="Q44" s="35"/>
+      <c r="R44" s="35"/>
+      <c r="S44" s="35"/>
+      <c r="T44" s="35"/>
+      <c r="U44" s="35"/>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="M45">
         <v>42</v>
       </c>
-      <c r="N45" s="41" t="s">
+      <c r="N45" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="O45" s="41"/>
-      <c r="P45" s="41"/>
-      <c r="Q45" s="41"/>
-      <c r="R45" s="41"/>
-      <c r="S45" s="41"/>
-      <c r="T45" s="41"/>
-      <c r="U45" s="41"/>
-    </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O45" s="35"/>
+      <c r="P45" s="35"/>
+      <c r="Q45" s="35"/>
+      <c r="R45" s="35"/>
+      <c r="S45" s="35"/>
+      <c r="T45" s="35"/>
+      <c r="U45" s="35"/>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="N46" s="36" t="s">
         <v>71</v>
       </c>
@@ -3594,7 +3601,7 @@
       <c r="T46" s="36"/>
       <c r="U46" s="36"/>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="N47" s="34"/>
       <c r="O47" s="34"/>
       <c r="P47" s="34"/>
@@ -3604,7 +3611,7 @@
       <c r="T47" s="34"/>
       <c r="U47" s="34"/>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="N48" s="34"/>
       <c r="O48" s="34"/>
       <c r="P48" s="34"/>
@@ -3614,7 +3621,7 @@
       <c r="T48" s="34"/>
       <c r="U48" s="34"/>
     </row>
-    <row r="49" spans="14:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N49" s="34"/>
       <c r="O49" s="34"/>
       <c r="P49" s="34"/>
@@ -3624,7 +3631,7 @@
       <c r="T49" s="34"/>
       <c r="U49" s="34"/>
     </row>
-    <row r="50" spans="14:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N50" s="34"/>
       <c r="O50" s="34"/>
       <c r="P50" s="34"/>
@@ -3634,7 +3641,7 @@
       <c r="T50" s="34"/>
       <c r="U50" s="34"/>
     </row>
-    <row r="51" spans="14:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N51" s="34"/>
       <c r="O51" s="34"/>
       <c r="P51" s="34"/>
@@ -3644,7 +3651,7 @@
       <c r="T51" s="34"/>
       <c r="U51" s="34"/>
     </row>
-    <row r="52" spans="14:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N52" s="34"/>
       <c r="O52" s="34"/>
       <c r="P52" s="34"/>
@@ -3654,7 +3661,7 @@
       <c r="T52" s="34"/>
       <c r="U52" s="34"/>
     </row>
-    <row r="53" spans="14:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="14:21" x14ac:dyDescent="0.25">
       <c r="N53" s="34"/>
       <c r="O53" s="34"/>
       <c r="P53" s="34"/>
@@ -3666,74 +3673,6 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="N49:U49"/>
-    <mergeCell ref="N50:U50"/>
-    <mergeCell ref="N51:U51"/>
-    <mergeCell ref="N52:U52"/>
-    <mergeCell ref="N53:U53"/>
-    <mergeCell ref="N44:U44"/>
-    <mergeCell ref="N45:U45"/>
-    <mergeCell ref="N46:U46"/>
-    <mergeCell ref="N47:U47"/>
-    <mergeCell ref="N48:U48"/>
-    <mergeCell ref="N39:U39"/>
-    <mergeCell ref="N40:U40"/>
-    <mergeCell ref="N41:U41"/>
-    <mergeCell ref="N42:U42"/>
-    <mergeCell ref="N43:U43"/>
-    <mergeCell ref="N34:U34"/>
-    <mergeCell ref="N35:U35"/>
-    <mergeCell ref="N36:U36"/>
-    <mergeCell ref="N37:U37"/>
-    <mergeCell ref="N38:U38"/>
-    <mergeCell ref="N29:U29"/>
-    <mergeCell ref="N30:U30"/>
-    <mergeCell ref="N31:U31"/>
-    <mergeCell ref="N32:U32"/>
-    <mergeCell ref="N33:U33"/>
-    <mergeCell ref="N24:U24"/>
-    <mergeCell ref="N25:U25"/>
-    <mergeCell ref="N26:U26"/>
-    <mergeCell ref="N27:U27"/>
-    <mergeCell ref="N28:U28"/>
-    <mergeCell ref="N19:U19"/>
-    <mergeCell ref="N20:U20"/>
-    <mergeCell ref="N21:U21"/>
-    <mergeCell ref="N22:U22"/>
-    <mergeCell ref="N23:U23"/>
-    <mergeCell ref="N14:U14"/>
-    <mergeCell ref="N15:U15"/>
-    <mergeCell ref="N16:U16"/>
-    <mergeCell ref="N17:U17"/>
-    <mergeCell ref="N18:U18"/>
-    <mergeCell ref="N9:U9"/>
-    <mergeCell ref="N10:U10"/>
-    <mergeCell ref="N11:U11"/>
-    <mergeCell ref="N12:U12"/>
-    <mergeCell ref="N13:U13"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="N4:U4"/>
-    <mergeCell ref="N5:U5"/>
-    <mergeCell ref="N6:U6"/>
-    <mergeCell ref="N7:U7"/>
-    <mergeCell ref="N8:U8"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B23:I23"/>
     <mergeCell ref="B32:I32"/>
     <mergeCell ref="B33:I33"/>
     <mergeCell ref="B34:I34"/>
@@ -3750,6 +3689,74 @@
     <mergeCell ref="B24:I24"/>
     <mergeCell ref="B25:I25"/>
     <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="N4:U4"/>
+    <mergeCell ref="N5:U5"/>
+    <mergeCell ref="N6:U6"/>
+    <mergeCell ref="N7:U7"/>
+    <mergeCell ref="N8:U8"/>
+    <mergeCell ref="N9:U9"/>
+    <mergeCell ref="N10:U10"/>
+    <mergeCell ref="N11:U11"/>
+    <mergeCell ref="N12:U12"/>
+    <mergeCell ref="N13:U13"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="N15:U15"/>
+    <mergeCell ref="N16:U16"/>
+    <mergeCell ref="N17:U17"/>
+    <mergeCell ref="N18:U18"/>
+    <mergeCell ref="N19:U19"/>
+    <mergeCell ref="N20:U20"/>
+    <mergeCell ref="N21:U21"/>
+    <mergeCell ref="N22:U22"/>
+    <mergeCell ref="N23:U23"/>
+    <mergeCell ref="N24:U24"/>
+    <mergeCell ref="N25:U25"/>
+    <mergeCell ref="N26:U26"/>
+    <mergeCell ref="N27:U27"/>
+    <mergeCell ref="N28:U28"/>
+    <mergeCell ref="N29:U29"/>
+    <mergeCell ref="N30:U30"/>
+    <mergeCell ref="N31:U31"/>
+    <mergeCell ref="N32:U32"/>
+    <mergeCell ref="N33:U33"/>
+    <mergeCell ref="N34:U34"/>
+    <mergeCell ref="N35:U35"/>
+    <mergeCell ref="N36:U36"/>
+    <mergeCell ref="N37:U37"/>
+    <mergeCell ref="N38:U38"/>
+    <mergeCell ref="N39:U39"/>
+    <mergeCell ref="N40:U40"/>
+    <mergeCell ref="N41:U41"/>
+    <mergeCell ref="N42:U42"/>
+    <mergeCell ref="N43:U43"/>
+    <mergeCell ref="N44:U44"/>
+    <mergeCell ref="N45:U45"/>
+    <mergeCell ref="N46:U46"/>
+    <mergeCell ref="N47:U47"/>
+    <mergeCell ref="N48:U48"/>
+    <mergeCell ref="N49:U49"/>
+    <mergeCell ref="N50:U50"/>
+    <mergeCell ref="N51:U51"/>
+    <mergeCell ref="N52:U52"/>
+    <mergeCell ref="N53:U53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3763,287 +3770,287 @@
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="7.1640625" customWidth="1"/>
-    <col min="19" max="19" width="20.83203125" customWidth="1"/>
+    <col min="11" max="11" width="7.125" customWidth="1"/>
+    <col min="19" max="19" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="L5" s="35" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L5" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="L6" s="45" t="s">
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="L6" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="50"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="L7" s="45" t="s">
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="L7" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="L8" s="37" t="s">
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="L8" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="L9" s="37" t="s">
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="L9" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="L10" s="37" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="L10" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="39"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="L11" s="37" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="L11" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="L12" s="37" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="L12" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="37"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="L13" s="37" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="L13" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="L16" s="37" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="L16" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="37"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="L17" s="37" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="L17" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -4052,50 +4059,50 @@
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="L19" s="37" t="s">
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="39"/>
+      <c r="S18" s="39"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L19" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="37"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="35" t="s">
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="L20" s="37" t="s">
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="L20" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>30</v>
       </c>
@@ -4106,18 +4113,18 @@
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="46"/>
-      <c r="Q21" s="46"/>
-      <c r="R21" s="46"/>
-      <c r="S21" s="46"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>34</v>
       </c>
@@ -4128,18 +4135,18 @@
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
       <c r="H22" s="34"/>
-      <c r="L22" s="46" t="s">
+      <c r="L22" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="46"/>
-      <c r="Q22" s="46"/>
-      <c r="R22" s="46"/>
-      <c r="S22" s="46"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>31</v>
       </c>
@@ -4150,18 +4157,18 @@
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
-      <c r="L23" s="50" t="s">
+      <c r="L23" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="50"/>
-      <c r="S23" s="50"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44"/>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="44"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>35</v>
       </c>
@@ -4173,7 +4180,7 @@
       <c r="G24" s="34"/>
       <c r="H24" s="34"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
         <v>32</v>
       </c>
@@ -4185,7 +4192,7 @@
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
         <v>36</v>
       </c>
@@ -4207,7 +4214,7 @@
       <c r="R26" s="34"/>
       <c r="S26" s="34"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
         <v>37</v>
       </c>
@@ -4218,18 +4225,18 @@
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
-      <c r="M27" s="42" t="s">
+      <c r="M27" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N27" s="48"/>
+      <c r="O27" s="48"/>
+      <c r="P27" s="48"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="48"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
@@ -4238,50 +4245,50 @@
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
-      <c r="M28" s="42" t="s">
+      <c r="M28" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="N28" s="42"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="42"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="48"/>
+      <c r="T28" s="48"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="M29" s="42" t="s">
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="M29" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="42"/>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="37" t="s">
+      <c r="N29" s="48"/>
+      <c r="O29" s="48"/>
+      <c r="P29" s="48"/>
+      <c r="Q29" s="48"/>
+      <c r="R29" s="48"/>
+      <c r="S29" s="48"/>
+      <c r="T29" s="48"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
       <c r="M30" s="47" t="s">
         <v>71</v>
       </c>
@@ -4293,29 +4300,29 @@
       <c r="S30" s="47"/>
       <c r="T30" s="47"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="37" t="s">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="M31" s="48" t="s">
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="M31" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
       <c r="T31" s="13"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -4327,6 +4334,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="M27:T27"/>
+    <mergeCell ref="M28:T28"/>
+    <mergeCell ref="M29:T29"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="L7:S7"/>
+    <mergeCell ref="L8:S8"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="L6:S6"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="L18:S18"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="L21:S21"/>
+    <mergeCell ref="L22:S22"/>
+    <mergeCell ref="L14:S14"/>
+    <mergeCell ref="L15:S15"/>
+    <mergeCell ref="L16:S16"/>
+    <mergeCell ref="L19:S19"/>
+    <mergeCell ref="L20:S20"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="L17:S17"/>
+    <mergeCell ref="M30:T30"/>
     <mergeCell ref="M31:S31"/>
     <mergeCell ref="L23:S23"/>
     <mergeCell ref="L5:S5"/>
@@ -4343,39 +4383,6 @@
     <mergeCell ref="L11:S11"/>
     <mergeCell ref="L12:S12"/>
     <mergeCell ref="L26:S26"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="L18:S18"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="L21:S21"/>
-    <mergeCell ref="L22:S22"/>
-    <mergeCell ref="L14:S14"/>
-    <mergeCell ref="L15:S15"/>
-    <mergeCell ref="L16:S16"/>
-    <mergeCell ref="L19:S19"/>
-    <mergeCell ref="L20:S20"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="L17:S17"/>
-    <mergeCell ref="M30:T30"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="M27:T27"/>
-    <mergeCell ref="M28:T28"/>
-    <mergeCell ref="M29:T29"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="L7:S7"/>
-    <mergeCell ref="L8:S8"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="L6:S6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4389,85 +4396,85 @@
       <selection activeCell="L14" sqref="L14:R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
     <col min="3" max="3" width="32.5" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.875" customWidth="1"/>
+    <col min="7" max="7" width="18.625" customWidth="1"/>
+    <col min="8" max="8" width="17.875" customWidth="1"/>
     <col min="11" max="11" width="7" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13.875" customWidth="1"/>
     <col min="18" max="18" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
       <c r="I2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
       <c r="S2" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
       <c r="I3">
         <v>4</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="L3" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
       <c r="S3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4499,7 +4506,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4531,7 +4538,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4563,7 +4570,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4595,7 +4602,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4627,7 +4634,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4659,7 +4666,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4691,7 +4698,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4710,20 +4717,20 @@
       <c r="K11">
         <v>9</v>
       </c>
-      <c r="L11" s="35" t="s">
+      <c r="L11" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
       <c r="S11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4755,19 +4762,19 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
       <c r="I13">
         <v>4</v>
       </c>
@@ -4787,19 +4794,19 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
       <c r="I14">
         <v>4</v>
       </c>
@@ -4819,7 +4826,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4844,7 +4851,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4862,7 +4869,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -4881,7 +4888,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -4893,19 +4900,19 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="15" t="s">
         <v>5</v>
       </c>
@@ -4913,7 +4920,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -4930,7 +4937,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -4947,7 +4954,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -4964,7 +4971,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -4981,7 +4988,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -4998,7 +5005,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -5015,7 +5022,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -5032,7 +5039,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8</v>
       </c>
@@ -5049,7 +5056,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9</v>
       </c>
@@ -5066,7 +5073,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
@@ -5083,7 +5090,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>11</v>
       </c>
@@ -5100,7 +5107,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>12</v>
       </c>
@@ -5117,7 +5124,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>13</v>
       </c>
@@ -5134,7 +5141,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>14</v>
       </c>
@@ -5151,35 +5158,35 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="52" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
       <c r="I34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="52" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="C35" s="52"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
       <c r="I35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="34"/>
       <c r="C36" s="34"/>
       <c r="D36" s="34"/>
@@ -5190,6 +5197,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="L3:R3"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="L6:R6"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="L8:R8"/>
+    <mergeCell ref="L9:R9"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="B36:H36"/>
     <mergeCell ref="L7:R7"/>
@@ -5206,38 +5245,6 @@
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="B33:H33"/>
     <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="L8:R8"/>
-    <mergeCell ref="L9:R9"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="L3:R3"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="L6:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>